<commit_message>
Sass eringefietst, opgeruimd, theme selecteren
</commit_message>
<xml_diff>
--- a/Rubric_WEBS6_1516D.xlsx
+++ b/Rubric_WEBS6_1516D.xlsx
@@ -830,14 +830,176 @@
     <xf numFmtId="1" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
@@ -845,173 +1007,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1408,8 +1408,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27:C29"/>
+      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,33 +1424,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="100" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="84"/>
+      <c r="B1" s="100"/>
       <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="84"/>
+      <c r="B2" s="100"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="100" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="84"/>
+      <c r="B3" s="100"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="58.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="85" t="s">
+      <c r="A4" s="101" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="85"/>
+      <c r="B4" s="101"/>
       <c r="C4" s="21"/>
       <c r="D4" s="46"/>
       <c r="E4" s="24" t="str">
@@ -1466,10 +1466,10 @@
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="107" t="s">
+      <c r="B5" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="108"/>
+      <c r="C5" s="69"/>
       <c r="D5" s="45">
         <v>8</v>
       </c>
@@ -1482,13 +1482,13 @@
       <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="86" t="s">
+      <c r="A6" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="111" t="s">
+      <c r="B6" s="72" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="112"/>
+      <c r="C6" s="73"/>
       <c r="D6" s="53">
         <v>1</v>
       </c>
@@ -1497,11 +1497,11 @@
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="87"/>
-      <c r="B7" s="113" t="s">
+      <c r="A7" s="103"/>
+      <c r="B7" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="114"/>
+      <c r="C7" s="75"/>
       <c r="D7" s="53">
         <v>1</v>
       </c>
@@ -1510,11 +1510,11 @@
       <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="87"/>
-      <c r="B8" s="113" t="s">
+      <c r="A8" s="103"/>
+      <c r="B8" s="74" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="114"/>
+      <c r="C8" s="75"/>
       <c r="D8" s="53">
         <v>1</v>
       </c>
@@ -1523,11 +1523,11 @@
       <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
-      <c r="B9" s="115" t="s">
+      <c r="A9" s="104"/>
+      <c r="B9" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="116"/>
+      <c r="C9" s="77"/>
       <c r="D9" s="54">
         <v>1</v>
       </c>
@@ -1539,13 +1539,13 @@
       <c r="G9" s="40"/>
     </row>
     <row r="10" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="124"/>
+      <c r="B10" s="66" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="67"/>
       <c r="D10" s="55">
         <v>10</v>
       </c>
@@ -1553,33 +1553,33 @@
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="123" t="s">
+      <c r="A11" s="64"/>
+      <c r="B11" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="124"/>
+      <c r="C11" s="67"/>
       <c r="D11" s="55">
         <v>10</v>
       </c>
       <c r="E11" s="27"/>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="123" t="s">
+      <c r="A12" s="64"/>
+      <c r="B12" s="66" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="124"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="55">
         <v>10</v>
       </c>
       <c r="E12" s="27"/>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="66"/>
-      <c r="B13" s="109" t="s">
+      <c r="A13" s="65"/>
+      <c r="B13" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="110"/>
+      <c r="C13" s="71"/>
       <c r="D13" s="56">
         <v>10</v>
       </c>
@@ -1594,35 +1594,35 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="80" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="104"/>
+      <c r="C14" s="81"/>
       <c r="D14" s="46">
         <v>10</v>
       </c>
       <c r="E14" s="28"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
-      <c r="B15" s="103" t="s">
+      <c r="A15" s="64"/>
+      <c r="B15" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="104"/>
+      <c r="C15" s="81"/>
       <c r="D15" s="46">
         <v>10</v>
       </c>
       <c r="E15" s="27"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="66"/>
-      <c r="B16" s="105" t="s">
+      <c r="A16" s="65"/>
+      <c r="B16" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="106"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="56">
         <v>10</v>
       </c>
@@ -1637,13 +1637,13 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65" t="s">
+      <c r="A17" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="101" t="s">
+      <c r="B17" s="78" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="102"/>
+      <c r="C17" s="79"/>
       <c r="D17" s="46">
         <v>10</v>
       </c>
@@ -1651,55 +1651,55 @@
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
-      <c r="B18" s="101" t="s">
+      <c r="A18" s="64"/>
+      <c r="B18" s="78" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="102"/>
+      <c r="C18" s="79"/>
       <c r="D18" s="46">
         <v>10</v>
       </c>
       <c r="E18" s="27"/>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="65"/>
-      <c r="B19" s="101" t="s">
+      <c r="A19" s="64"/>
+      <c r="B19" s="78" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="102"/>
+      <c r="C19" s="79"/>
       <c r="D19" s="46">
         <v>10</v>
       </c>
       <c r="E19" s="27"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="65"/>
-      <c r="B20" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="96"/>
+      <c r="A20" s="64"/>
+      <c r="B20" s="88" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="89"/>
       <c r="D20" s="57">
         <v>10</v>
       </c>
       <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
-      <c r="B21" s="97" t="s">
+      <c r="A21" s="64"/>
+      <c r="B21" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="98"/>
+      <c r="C21" s="91"/>
       <c r="D21" s="57">
         <v>10</v>
       </c>
       <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="66"/>
-      <c r="B22" s="99" t="s">
+      <c r="A22" s="65"/>
+      <c r="B22" s="92" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="100"/>
+      <c r="C22" s="93"/>
       <c r="D22" s="58">
         <v>10</v>
       </c>
@@ -1714,13 +1714,13 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65" t="s">
+      <c r="A23" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="89" t="s">
+      <c r="B23" s="84" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="90"/>
+      <c r="C23" s="85"/>
       <c r="D23" s="46">
         <v>10</v>
       </c>
@@ -1728,33 +1728,33 @@
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
-      <c r="B24" s="89" t="s">
+      <c r="A24" s="64"/>
+      <c r="B24" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="90"/>
+      <c r="C24" s="85"/>
       <c r="D24" s="46">
         <v>10</v>
       </c>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
-      <c r="B25" s="89" t="s">
+      <c r="A25" s="64"/>
+      <c r="B25" s="84" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="90"/>
+      <c r="C25" s="85"/>
       <c r="D25" s="46">
         <v>10</v>
       </c>
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="66"/>
-      <c r="B26" s="93" t="s">
+      <c r="A26" s="65"/>
+      <c r="B26" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="94"/>
+      <c r="C26" s="87"/>
       <c r="D26" s="58">
         <v>10</v>
       </c>
@@ -1769,46 +1769,46 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="16.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65" t="s">
+      <c r="A27" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="89" t="s">
+      <c r="B27" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="90"/>
+      <c r="C27" s="79"/>
       <c r="D27" s="46">
         <v>10</v>
       </c>
       <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
-      <c r="B28" s="89" t="s">
+      <c r="A28" s="64"/>
+      <c r="B28" s="84" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="90"/>
+      <c r="C28" s="85"/>
       <c r="D28" s="46">
         <v>10</v>
       </c>
       <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
-      <c r="B29" s="89" t="s">
+      <c r="A29" s="64"/>
+      <c r="B29" s="84" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="90"/>
+      <c r="C29" s="85"/>
       <c r="D29" s="46">
         <v>10</v>
       </c>
       <c r="E29" s="27"/>
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="66"/>
-      <c r="B30" s="91" t="s">
+      <c r="A30" s="65"/>
+      <c r="B30" s="94" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="92"/>
+      <c r="C30" s="95"/>
       <c r="D30" s="58">
         <v>10</v>
       </c>
@@ -1823,68 +1823,68 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="73" t="s">
+      <c r="B31" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="74"/>
+      <c r="C31" s="111"/>
       <c r="D31" s="46">
         <v>10</v>
       </c>
       <c r="E31" s="27"/>
     </row>
     <row r="32" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="78" t="s">
+      <c r="A32" s="113"/>
+      <c r="B32" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="79"/>
+      <c r="C32" s="116"/>
       <c r="D32" s="47">
         <v>10</v>
       </c>
       <c r="E32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="76"/>
-      <c r="B33" s="80" t="s">
+      <c r="A33" s="113"/>
+      <c r="B33" s="117" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="81"/>
+      <c r="C33" s="118"/>
       <c r="D33" s="47">
         <v>10</v>
       </c>
       <c r="E33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="76"/>
-      <c r="B34" s="80" t="s">
+      <c r="A34" s="113"/>
+      <c r="B34" s="117" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="81"/>
+      <c r="C34" s="118"/>
       <c r="D34" s="47">
         <v>10</v>
       </c>
       <c r="E34" s="27"/>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="76"/>
-      <c r="B35" s="80" t="s">
+      <c r="A35" s="113"/>
+      <c r="B35" s="117" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="81"/>
+      <c r="C35" s="118"/>
       <c r="D35" s="47">
         <v>10</v>
       </c>
       <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="77"/>
-      <c r="B36" s="82" t="s">
+      <c r="A36" s="114"/>
+      <c r="B36" s="119" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="83"/>
+      <c r="C36" s="120"/>
       <c r="D36" s="48">
         <v>10</v>
       </c>
@@ -1899,57 +1899,57 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="64" t="s">
+      <c r="A37" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="119" t="s">
+      <c r="B37" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="120"/>
+      <c r="C37" s="99"/>
       <c r="D37" s="46">
         <v>10</v>
       </c>
       <c r="E37" s="27"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="65"/>
-      <c r="B38" s="69" t="s">
+      <c r="A38" s="64"/>
+      <c r="B38" s="96" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="70"/>
+      <c r="C38" s="97"/>
       <c r="D38" s="47">
         <v>10</v>
       </c>
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="65"/>
-      <c r="B39" s="117" t="s">
+      <c r="A39" s="64"/>
+      <c r="B39" s="106" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="118"/>
+      <c r="C39" s="107"/>
       <c r="D39" s="47">
         <v>10</v>
       </c>
       <c r="E39" s="27"/>
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="65"/>
-      <c r="B40" s="117" t="s">
+      <c r="A40" s="64"/>
+      <c r="B40" s="106" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="118"/>
+      <c r="C40" s="107"/>
       <c r="D40" s="47">
         <v>10</v>
       </c>
       <c r="E40" s="27"/>
     </row>
     <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="66"/>
-      <c r="B41" s="121" t="s">
+      <c r="A41" s="65"/>
+      <c r="B41" s="108" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="122"/>
+      <c r="C41" s="109"/>
       <c r="D41" s="49">
         <v>10</v>
       </c>
@@ -1964,13 +1964,13 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="64" t="s">
+      <c r="A42" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="67" t="s">
+      <c r="B42" s="121" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="68"/>
+      <c r="C42" s="122"/>
       <c r="D42" s="50">
         <v>10</v>
       </c>
@@ -1978,11 +1978,11 @@
       <c r="F42" s="14"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="65"/>
-      <c r="B43" s="69" t="s">
+      <c r="A43" s="64"/>
+      <c r="B43" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="70"/>
+      <c r="C43" s="97"/>
       <c r="D43" s="47">
         <v>10</v>
       </c>
@@ -1990,17 +1990,17 @@
       <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="65"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="70"/>
+      <c r="A44" s="64"/>
+      <c r="B44" s="96"/>
+      <c r="C44" s="97"/>
       <c r="D44" s="47"/>
       <c r="E44" s="35"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="66"/>
-      <c r="B45" s="71"/>
-      <c r="C45" s="72"/>
+      <c r="A45" s="65"/>
+      <c r="B45" s="123"/>
+      <c r="C45" s="124"/>
       <c r="D45" s="49"/>
       <c r="E45" s="30"/>
       <c r="F45" s="36">
@@ -2216,44 +2216,11 @@
     </row>
   </sheetData>
   <mergeCells count="54">
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
@@ -2265,11 +2232,44 @@
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
     <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="A17:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A30"/>
   </mergeCells>
   <conditionalFormatting sqref="E4">
     <cfRule type="cellIs" dxfId="5" priority="6" operator="lessThan">

</xml_diff>

<commit_message>
Tests af plus laatste loodjes
</commit_message>
<xml_diff>
--- a/Rubric_WEBS6_1516D.xlsx
+++ b/Rubric_WEBS6_1516D.xlsx
@@ -386,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,12 +423,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -651,7 +645,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="125">
+  <cellXfs count="117">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -836,10 +830,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -848,10 +842,10 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
@@ -872,23 +866,29 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <alignment vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
@@ -896,46 +896,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -956,22 +926,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -983,22 +953,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1012,6 +970,18 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1408,8 +1378,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29:C29"/>
+      <pane ySplit="4" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1424,38 +1394,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A1" s="100" t="s">
+      <c r="A1" s="92" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="100"/>
+      <c r="B1" s="92"/>
       <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
+      <c r="A2" s="92" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="100"/>
+      <c r="B2" s="92"/>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:11" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="100"/>
+      <c r="B3" s="92"/>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="58.9" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="101" t="s">
+      <c r="A4" s="93" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="101"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="21"/>
       <c r="D4" s="46"/>
-      <c r="E4" s="24" t="str">
+      <c r="E4" s="24">
         <f>IF(SUM(E6:E9)&lt;4, "NB", E55)</f>
-        <v>NB</v>
+        <v>7.8083333333333336</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="41"/>
@@ -1482,7 +1452,7 @@
       <c r="I5" s="31"/>
     </row>
     <row r="6" spans="1:11" s="1" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="102" t="s">
+      <c r="A6" s="94" t="s">
         <v>28</v>
       </c>
       <c r="B6" s="72" t="s">
@@ -1492,12 +1462,14 @@
       <c r="D6" s="53">
         <v>1</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="25">
+        <v>1</v>
+      </c>
       <c r="F6" s="10"/>
       <c r="G6" s="40"/>
     </row>
     <row r="7" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="103"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="74" t="s">
         <v>35</v>
       </c>
@@ -1505,12 +1477,14 @@
       <c r="D7" s="53">
         <v>1</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="25">
+        <v>1</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="40"/>
     </row>
     <row r="8" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="74" t="s">
         <v>36</v>
       </c>
@@ -1518,12 +1492,14 @@
       <c r="D8" s="53">
         <v>1</v>
       </c>
-      <c r="E8" s="25"/>
+      <c r="E8" s="25">
+        <v>1</v>
+      </c>
       <c r="F8" s="10"/>
       <c r="G8" s="40"/>
     </row>
     <row r="9" spans="1:11" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="104"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="76" t="s">
         <v>37</v>
       </c>
@@ -1531,10 +1507,12 @@
       <c r="D9" s="54">
         <v>1</v>
       </c>
-      <c r="E9" s="26"/>
+      <c r="E9" s="26">
+        <v>1</v>
+      </c>
       <c r="F9" s="11" t="str">
         <f>IF(SUM(E6:E9)&lt;SUM(D6:D9), "KO", "OK")</f>
-        <v>KO</v>
+        <v>OK</v>
       </c>
       <c r="G9" s="40"/>
     </row>
@@ -1549,7 +1527,9 @@
       <c r="D10" s="55">
         <v>10</v>
       </c>
-      <c r="E10" s="27"/>
+      <c r="E10" s="27">
+        <v>10</v>
+      </c>
       <c r="F10" s="12"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
@@ -1561,7 +1541,9 @@
       <c r="D11" s="55">
         <v>10</v>
       </c>
-      <c r="E11" s="27"/>
+      <c r="E11" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="64"/>
@@ -1572,7 +1554,9 @@
       <c r="D12" s="55">
         <v>10</v>
       </c>
-      <c r="E12" s="27"/>
+      <c r="E12" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="65"/>
@@ -1583,10 +1567,12 @@
       <c r="D13" s="56">
         <v>10</v>
       </c>
-      <c r="E13" s="27"/>
+      <c r="E13" s="27">
+        <v>10</v>
+      </c>
       <c r="F13" s="13">
         <f>SUM(E10:E13)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G13" s="42">
         <f>SUM(D10:D13)</f>
@@ -1604,7 +1590,9 @@
       <c r="D14" s="46">
         <v>10</v>
       </c>
-      <c r="E14" s="28"/>
+      <c r="E14" s="28">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="64"/>
@@ -1615,21 +1603,23 @@
       <c r="D15" s="46">
         <v>10</v>
       </c>
-      <c r="E15" s="27"/>
+      <c r="E15" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
-      <c r="B16" s="82" t="s">
+      <c r="B16" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="83"/>
+      <c r="C16" s="114"/>
       <c r="D16" s="56">
         <v>10</v>
       </c>
       <c r="E16" s="29"/>
       <c r="F16" s="10">
         <f>SUM(E14:E16)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G16" s="42">
         <f>SUM(D14:D16)</f>
@@ -1647,7 +1637,9 @@
       <c r="D17" s="46">
         <v>10</v>
       </c>
-      <c r="E17" s="28"/>
+      <c r="E17" s="28">
+        <v>10</v>
+      </c>
       <c r="F17" s="12"/>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1659,7 +1651,9 @@
       <c r="D18" s="46">
         <v>10</v>
       </c>
-      <c r="E18" s="27"/>
+      <c r="E18" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="64"/>
@@ -1670,43 +1664,51 @@
       <c r="D19" s="46">
         <v>10</v>
       </c>
-      <c r="E19" s="27"/>
+      <c r="E19" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="64"/>
-      <c r="B20" s="88" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="89"/>
+      <c r="B20" s="78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="79"/>
       <c r="D20" s="57">
         <v>10</v>
       </c>
-      <c r="E20" s="27"/>
+      <c r="E20" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
-      <c r="B21" s="90" t="s">
+      <c r="B21" s="84" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="91"/>
+      <c r="C21" s="85"/>
       <c r="D21" s="57">
         <v>10</v>
       </c>
-      <c r="E21" s="27"/>
+      <c r="E21" s="27">
+        <v>5</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="65"/>
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="82" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="93"/>
+      <c r="C22" s="83"/>
       <c r="D22" s="58">
         <v>10</v>
       </c>
-      <c r="E22" s="27"/>
+      <c r="E22" s="27">
+        <v>10</v>
+      </c>
       <c r="F22" s="10">
         <f>SUM(E17:E22)</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="G22" s="42">
         <f>SUM(D17:D22)</f>
@@ -1717,51 +1719,59 @@
       <c r="A23" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B23" s="84" t="s">
+      <c r="B23" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="85"/>
+      <c r="C23" s="79"/>
       <c r="D23" s="46">
         <v>10</v>
       </c>
-      <c r="E23" s="28"/>
+      <c r="E23" s="28">
+        <v>10</v>
+      </c>
       <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="64"/>
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="85"/>
+      <c r="C24" s="79"/>
       <c r="D24" s="46">
         <v>10</v>
       </c>
-      <c r="E24" s="27"/>
+      <c r="E24" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="64"/>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="85"/>
+      <c r="C25" s="79"/>
       <c r="D25" s="46">
         <v>10</v>
       </c>
-      <c r="E25" s="27"/>
+      <c r="E25" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="65"/>
-      <c r="B26" s="86" t="s">
+      <c r="B26" s="82" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="87"/>
+      <c r="C26" s="83"/>
       <c r="D26" s="58">
         <v>10</v>
       </c>
-      <c r="E26" s="27"/>
+      <c r="E26" s="27">
+        <v>10</v>
+      </c>
       <c r="F26" s="13">
         <f>SUM(E23:E26)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G26" s="42">
         <f>SUM(D23:D26)</f>
@@ -1779,14 +1789,16 @@
       <c r="D27" s="46">
         <v>10</v>
       </c>
-      <c r="E27" s="28"/>
+      <c r="E27" s="28">
+        <v>10</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="64"/>
-      <c r="B28" s="84" t="s">
+      <c r="B28" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="C28" s="85"/>
+      <c r="C28" s="87"/>
       <c r="D28" s="46">
         <v>10</v>
       </c>
@@ -1794,10 +1806,10 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="64"/>
-      <c r="B29" s="84" t="s">
+      <c r="B29" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="85"/>
+      <c r="C29" s="87"/>
       <c r="D29" s="46">
         <v>10</v>
       </c>
@@ -1805,17 +1817,19 @@
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="65"/>
-      <c r="B30" s="94" t="s">
+      <c r="B30" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="95"/>
+      <c r="C30" s="83"/>
       <c r="D30" s="58">
         <v>10</v>
       </c>
-      <c r="E30" s="30"/>
+      <c r="E30" s="30">
+        <v>10</v>
+      </c>
       <c r="F30" s="13">
         <f>SUM(E27:E30)</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G30" s="42">
         <f>SUM(D27:D30)</f>
@@ -1823,75 +1837,87 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="112" t="s">
+      <c r="A31" s="104" t="s">
         <v>26</v>
       </c>
-      <c r="B31" s="110" t="s">
+      <c r="B31" s="102" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="111"/>
+      <c r="C31" s="103"/>
       <c r="D31" s="46">
         <v>10</v>
       </c>
-      <c r="E31" s="27"/>
+      <c r="E31" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="113"/>
-      <c r="B32" s="115" t="s">
+      <c r="A32" s="105"/>
+      <c r="B32" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="C32" s="116"/>
+      <c r="C32" s="108"/>
       <c r="D32" s="47">
         <v>10</v>
       </c>
-      <c r="E32" s="27"/>
+      <c r="E32" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="113"/>
-      <c r="B33" s="117" t="s">
+      <c r="A33" s="105"/>
+      <c r="B33" s="107" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="118"/>
+      <c r="C33" s="108"/>
       <c r="D33" s="47">
         <v>10</v>
       </c>
-      <c r="E33" s="27"/>
+      <c r="E33" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="34" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="113"/>
-      <c r="B34" s="117" t="s">
+      <c r="A34" s="105"/>
+      <c r="B34" s="107" t="s">
         <v>42</v>
       </c>
-      <c r="C34" s="118"/>
+      <c r="C34" s="108"/>
       <c r="D34" s="47">
         <v>10</v>
       </c>
-      <c r="E34" s="27"/>
+      <c r="E34" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="117" t="s">
+      <c r="A35" s="105"/>
+      <c r="B35" s="107" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="118"/>
+      <c r="C35" s="108"/>
       <c r="D35" s="47">
         <v>10</v>
       </c>
-      <c r="E35" s="27"/>
+      <c r="E35" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="114"/>
-      <c r="B36" s="119" t="s">
+      <c r="A36" s="106"/>
+      <c r="B36" s="115" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="120"/>
+      <c r="C36" s="116"/>
       <c r="D36" s="48">
         <v>10</v>
       </c>
-      <c r="E36" s="30"/>
+      <c r="E36" s="30">
+        <v>10</v>
+      </c>
       <c r="F36" s="38">
         <f>SUM(E31:E36)</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="G36" s="42">
         <f>SUM(D31:D36)</f>
@@ -1899,24 +1925,26 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="105" t="s">
+      <c r="A37" s="97" t="s">
         <v>27</v>
       </c>
-      <c r="B37" s="98" t="s">
+      <c r="B37" s="90" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="99"/>
+      <c r="C37" s="91"/>
       <c r="D37" s="46">
         <v>10</v>
       </c>
-      <c r="E37" s="27"/>
+      <c r="E37" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="64"/>
-      <c r="B38" s="96" t="s">
+      <c r="B38" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="97"/>
+      <c r="C38" s="89"/>
       <c r="D38" s="47">
         <v>10</v>
       </c>
@@ -1924,39 +1952,45 @@
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="64"/>
-      <c r="B39" s="106" t="s">
+      <c r="B39" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="C39" s="107"/>
+      <c r="C39" s="99"/>
       <c r="D39" s="47">
         <v>10</v>
       </c>
-      <c r="E39" s="27"/>
+      <c r="E39" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="64"/>
-      <c r="B40" s="106" t="s">
+      <c r="B40" s="98" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="107"/>
+      <c r="C40" s="99"/>
       <c r="D40" s="47">
         <v>10</v>
       </c>
-      <c r="E40" s="27"/>
+      <c r="E40" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="41" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="65"/>
-      <c r="B41" s="108" t="s">
+      <c r="B41" s="100" t="s">
         <v>50</v>
       </c>
-      <c r="C41" s="109"/>
+      <c r="C41" s="101"/>
       <c r="D41" s="49">
         <v>10</v>
       </c>
-      <c r="E41" s="30"/>
+      <c r="E41" s="30">
+        <v>10</v>
+      </c>
       <c r="F41" s="37">
         <f>SUM(E37:E41)</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="G41" s="40">
         <f>SUM(D37:D41)</f>
@@ -1964,13 +1998,13 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="105" t="s">
+      <c r="A42" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="121" t="s">
+      <c r="B42" s="109" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="122"/>
+      <c r="C42" s="110"/>
       <c r="D42" s="50">
         <v>10</v>
       </c>
@@ -1979,10 +2013,10 @@
     </row>
     <row r="43" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="64"/>
-      <c r="B43" s="96" t="s">
+      <c r="B43" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="C43" s="97"/>
+      <c r="C43" s="89"/>
       <c r="D43" s="47">
         <v>10</v>
       </c>
@@ -1991,16 +2025,16 @@
     </row>
     <row r="44" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="64"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="97"/>
+      <c r="B44" s="88"/>
+      <c r="C44" s="89"/>
       <c r="D44" s="47"/>
       <c r="E44" s="35"/>
       <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="65"/>
-      <c r="B45" s="123"/>
-      <c r="C45" s="124"/>
+      <c r="B45" s="111"/>
+      <c r="C45" s="112"/>
       <c r="D45" s="49"/>
       <c r="E45" s="30"/>
       <c r="F45" s="36">
@@ -2033,7 +2067,7 @@
       </c>
       <c r="B47" s="62">
         <f>F13</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>14</v>
@@ -2041,7 +2075,7 @@
       <c r="D47" s="51"/>
       <c r="E47" s="18">
         <f t="shared" ref="E47:E54" si="0">(B47  / A47 ) * F47 * 10</f>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F47" s="15">
         <v>0.05</v>
@@ -2054,7 +2088,7 @@
       </c>
       <c r="B48" s="62">
         <f>F16</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>15</v>
@@ -2062,7 +2096,7 @@
       <c r="D48" s="51"/>
       <c r="E48" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F48" s="15">
         <v>0.05</v>
@@ -2075,7 +2109,7 @@
       </c>
       <c r="B49" s="62">
         <f>F22</f>
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>16</v>
@@ -2083,7 +2117,7 @@
       <c r="D49" s="51"/>
       <c r="E49" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3749999999999998</v>
       </c>
       <c r="F49" s="15">
         <v>0.15</v>
@@ -2096,7 +2130,7 @@
       </c>
       <c r="B50" s="62">
         <f>F26</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>20</v>
@@ -2104,7 +2138,7 @@
       <c r="D50" s="51"/>
       <c r="E50" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F50" s="15">
         <v>0.15</v>
@@ -2117,7 +2151,7 @@
       </c>
       <c r="B51" s="62">
         <f>F30</f>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>25</v>
@@ -2125,7 +2159,7 @@
       <c r="D51" s="51"/>
       <c r="E51" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F51" s="15">
         <v>0.1</v>
@@ -2138,7 +2172,7 @@
       </c>
       <c r="B52" s="63">
         <f>F36</f>
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>26</v>
@@ -2146,7 +2180,7 @@
       <c r="D52" s="51"/>
       <c r="E52" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F52" s="15">
         <v>0.2</v>
@@ -2159,7 +2193,7 @@
       </c>
       <c r="B53" s="63">
         <f>F41</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>27</v>
@@ -2167,7 +2201,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.6000000000000003</v>
       </c>
       <c r="F53" s="15">
         <v>0.2</v>
@@ -2203,7 +2237,7 @@
       <c r="D55" s="46"/>
       <c r="E55" s="32">
         <f>SUM(E47:E54)</f>
-        <v>0</v>
+        <v>7.8083333333333336</v>
       </c>
       <c r="F55" s="23">
         <f>SUM(F47:F54)</f>

</xml_diff>

<commit_message>
Socket en verschillende stylehseets
</commit_message>
<xml_diff>
--- a/Rubric_WEBS6_1516D.xlsx
+++ b/Rubric_WEBS6_1516D.xlsx
@@ -386,7 +386,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -427,6 +427,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="18">
     <border>
@@ -878,18 +884,18 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" readingOrder="1"/>
     </xf>
@@ -959,6 +965,12 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
@@ -971,17 +983,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1378,8 +1384,8 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27:C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1425,7 +1431,7 @@
       <c r="D4" s="46"/>
       <c r="E4" s="24">
         <f>IF(SUM(E6:E9)&lt;4, "NB", E55)</f>
-        <v>7.8083333333333336</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="41"/>
@@ -1609,10 +1615,10 @@
     </row>
     <row r="16" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
-      <c r="B16" s="113" t="s">
+      <c r="B16" s="82" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="114"/>
+      <c r="C16" s="83"/>
       <c r="D16" s="56">
         <v>10</v>
       </c>
@@ -1683,23 +1689,23 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="64"/>
-      <c r="B21" s="84" t="s">
+      <c r="B21" s="78" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="85"/>
+      <c r="C21" s="79"/>
       <c r="D21" s="57">
         <v>10</v>
       </c>
       <c r="E21" s="27">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="65"/>
-      <c r="B22" s="82" t="s">
+      <c r="B22" s="84" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="83"/>
+      <c r="C22" s="85"/>
       <c r="D22" s="58">
         <v>10</v>
       </c>
@@ -1708,7 +1714,7 @@
       </c>
       <c r="F22" s="10">
         <f>SUM(E17:E22)</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="G22" s="42">
         <f>SUM(D17:D22)</f>
@@ -1759,10 +1765,10 @@
     </row>
     <row r="26" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="65"/>
-      <c r="B26" s="82" t="s">
+      <c r="B26" s="84" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="83"/>
+      <c r="C26" s="85"/>
       <c r="D26" s="58">
         <v>10</v>
       </c>
@@ -1782,10 +1788,10 @@
       <c r="A27" s="64" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="78" t="s">
+      <c r="B27" s="115" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="79"/>
+      <c r="C27" s="116"/>
       <c r="D27" s="46">
         <v>10</v>
       </c>
@@ -1817,10 +1823,10 @@
     </row>
     <row r="30" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="65"/>
-      <c r="B30" s="82" t="s">
+      <c r="B30" s="84" t="s">
         <v>24</v>
       </c>
-      <c r="C30" s="83"/>
+      <c r="C30" s="85"/>
       <c r="D30" s="58">
         <v>10</v>
       </c>
@@ -1905,10 +1911,10 @@
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="106"/>
-      <c r="B36" s="115" t="s">
+      <c r="B36" s="109" t="s">
         <v>44</v>
       </c>
-      <c r="C36" s="116"/>
+      <c r="C36" s="110"/>
       <c r="D36" s="48">
         <v>10</v>
       </c>
@@ -1941,14 +1947,16 @@
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="64"/>
-      <c r="B38" s="88" t="s">
+      <c r="B38" s="98" t="s">
         <v>48</v>
       </c>
-      <c r="C38" s="89"/>
+      <c r="C38" s="99"/>
       <c r="D38" s="47">
         <v>10</v>
       </c>
-      <c r="E38" s="27"/>
+      <c r="E38" s="27">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="64"/>
@@ -1990,7 +1998,7 @@
       </c>
       <c r="F41" s="37">
         <f>SUM(E37:E41)</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="G41" s="40">
         <f>SUM(D37:D41)</f>
@@ -2001,10 +2009,10 @@
       <c r="A42" s="97" t="s">
         <v>52</v>
       </c>
-      <c r="B42" s="109" t="s">
+      <c r="B42" s="111" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="110"/>
+      <c r="C42" s="112"/>
       <c r="D42" s="50">
         <v>10</v>
       </c>
@@ -2033,8 +2041,8 @@
     </row>
     <row r="45" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="65"/>
-      <c r="B45" s="111"/>
-      <c r="C45" s="112"/>
+      <c r="B45" s="113"/>
+      <c r="C45" s="114"/>
       <c r="D45" s="49"/>
       <c r="E45" s="30"/>
       <c r="F45" s="36">
@@ -2109,7 +2117,7 @@
       </c>
       <c r="B49" s="62">
         <f>F22</f>
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>16</v>
@@ -2117,7 +2125,7 @@
       <c r="D49" s="51"/>
       <c r="E49" s="18">
         <f t="shared" si="0"/>
-        <v>1.3749999999999998</v>
+        <v>1.5</v>
       </c>
       <c r="F49" s="15">
         <v>0.15</v>
@@ -2193,7 +2201,7 @@
       </c>
       <c r="B53" s="63">
         <f>F41</f>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>27</v>
@@ -2201,7 +2209,7 @@
       <c r="D53" s="51"/>
       <c r="E53" s="18">
         <f t="shared" si="0"/>
-        <v>1.6000000000000003</v>
+        <v>2</v>
       </c>
       <c r="F53" s="15">
         <v>0.2</v>
@@ -2237,7 +2245,7 @@
       <c r="D55" s="46"/>
       <c r="E55" s="32">
         <f>SUM(E47:E54)</f>
-        <v>7.8083333333333336</v>
+        <v>8.3333333333333321</v>
       </c>
       <c r="F55" s="23">
         <f>SUM(F47:F54)</f>

</xml_diff>